<commit_message>
se modifica modelo y se quita campo identity para tabla Version y Estructura
</commit_message>
<xml_diff>
--- a/branches/vidacamara_1/docs/bugs/informe_bugs.xlsx
+++ b/branches/vidacamara_1/docs/bugs/informe_bugs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="18855" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="18855" windowHeight="8190" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -15,14 +15,14 @@
     <sheet name="Hoja2" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Resumen!$A$2:$E$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Resumen!$A$2:$E$20</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="45">
   <si>
     <t>Descripción</t>
   </si>
@@ -139,13 +139,31 @@
   </si>
   <si>
     <t xml:space="preserve">sql server no poporta in de subselect, se comenta @Fetch(FetchMode.SUBSELECT) </t>
+  </si>
+  <si>
+    <t>Exportar a Word</t>
+  </si>
+  <si>
+    <t>Exportar a Excel</t>
+  </si>
+  <si>
+    <t>Historial Reporte</t>
+  </si>
+  <si>
+    <t>Varias</t>
+  </si>
+  <si>
+    <t>Se corrigen errores Variados</t>
+  </si>
+  <si>
+    <t>Evidencias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +188,14 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -212,13 +238,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -226,6 +253,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -426,6 +458,271 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>741335</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>142166</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="1 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect t="10236"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="790575" y="4972050"/>
+          <a:ext cx="12923810" cy="5095166"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>369903</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>75477</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="2 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="11049000"/>
+          <a:ext cx="12580953" cy="5790477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>570189</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>46929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="3 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="17716500"/>
+          <a:ext cx="10495239" cy="5571429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>150856</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>161238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="4 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="23622000"/>
+          <a:ext cx="12361906" cy="5495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>512951</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>132619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="5 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="29908500"/>
+          <a:ext cx="11200001" cy="5847619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>191</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>293713</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>37429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="6 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="36195000"/>
+          <a:ext cx="12504763" cy="5371429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>417481</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>94643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="7 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14144625" y="4762500"/>
+          <a:ext cx="12961906" cy="4857143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -504,6 +801,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -538,6 +836,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -713,21 +1012,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A2:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="84.140625" customWidth="1"/>
     <col min="3" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -744,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
@@ -761,7 +1061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -778,7 +1078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -795,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
@@ -812,7 +1112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
@@ -823,13 +1123,13 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
@@ -846,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
@@ -863,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
@@ -880,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -897,7 +1197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -914,7 +1214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
@@ -931,7 +1231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
@@ -948,7 +1248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
@@ -965,7 +1265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
@@ -976,13 +1276,13 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
@@ -999,7 +1299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
@@ -1016,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>34</v>
       </c>
@@ -1033,7 +1333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>35</v>
       </c>
@@ -1051,7 +1351,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E2"/>
+  <autoFilter ref="A2:E20">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="RRC"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="E6" location="flujo!A1" display="link"/>
     <hyperlink ref="E7" location="reportes!A1" display="link"/>
@@ -1064,20 +1370,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="87.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1085,7 +1391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>37</v>
       </c>
@@ -1100,20 +1406,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="105.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1121,7 +1427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -1136,19 +1442,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C157"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="68.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1156,31 +1462,66 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="58" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B58" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>